<commit_message>
Updated excel files used to calculate/verify motion parameters based on the values from embedded code.
</commit_message>
<xml_diff>
--- a/Doc/Measurements/Inter_Steps_Delay.xlsx
+++ b/Doc/Measurements/Inter_Steps_Delay.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\StepperMotorControl\Doc\Measurements\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8778175D-8389-47D4-A48F-6E7C38615FBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{972EE436-95BD-4B63-89D2-AA9DFF55B938}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +22,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ciprian salageanu</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ciprian salageanu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+distance (or displacement) is one motor step on each new motor command (step). For a motor with step of 1.8 degrees =&gt; 0.031416 radians.
+Speed is calculated by dividing the displacement by time (delay between two consecutive steps)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57,18 +86,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,8 +135,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,7 +155,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -157,6 +199,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -165,26 +208,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -194,7 +217,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
             <c:v>Time vs Step Number</c:v>
           </c:tx>
@@ -565,7 +588,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-B4BA-4F71-9876-1134AEF3471A}"/>
             </c:ext>
@@ -579,10 +602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="440759352"/>
-        <c:axId val="440756400"/>
-        <c:extLst>
+        <c:axId val="229471744"/>
+        <c:axId val="232478912"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -978,7 +1002,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="440759352"/>
+        <c:axId val="229471744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,6 +1039,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1023,26 +1048,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1081,7 +1086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440756400"/>
+        <c:crossAx val="232478912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1089,7 +1094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440756400"/>
+        <c:axId val="232478912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,6 +1154,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1157,26 +1163,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1209,7 +1195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440759352"/>
+        <c:crossAx val="229471744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1223,6 +1209,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1254,14 +1241,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1296,7 +1283,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1310,6 +1297,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1721,7 +1709,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000190-2774-46DA-B118-8B32812649E4}"/>
             </c:ext>
@@ -1735,11 +1723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="498066336"/>
-        <c:axId val="498065680"/>
+        <c:axId val="232980480"/>
+        <c:axId val="232981056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="498066336"/>
+        <c:axId val="232980480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,6 +1773,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1793,26 +1782,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1851,12 +1820,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="498065680"/>
+        <c:crossAx val="232981056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="498065680"/>
+        <c:axId val="232981056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1902,6 +1871,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1910,26 +1880,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1968,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="498066336"/>
+        <c:crossAx val="232980480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1982,14 +1932,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3156,7 +3106,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1BCD51-2584-4157-8F75-C8ACB057005F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0D1BCD51-2584-4157-8F75-C8ACB057005F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3311,7 +3261,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9D7135-AA9C-4261-826A-472856EB2B64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BE9D7135-AA9C-4261-826A-472856EB2B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3347,7 +3297,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89D6CF97-4BBF-48D8-B40C-0CA61767406B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89D6CF97-4BBF-48D8-B40C-0CA61767406B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3383,7 +3333,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FC4D125-7781-4A96-A021-6225D39C354C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1FC4D125-7781-4A96-A021-6225D39C354C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3741,18 +3691,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D165640-C44E-4B91-AA7F-8B17F0DDBC1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3884,7 +3834,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f>0.0314159265/E7</f>
         <v>0.66418449260042278</v>
       </c>
       <c r="W7" s="1">
@@ -5146,5 +5096,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>